<commit_message>
save now at remoing lecescy code
</commit_message>
<xml_diff>
--- a/result_test_full_features.xlsx
+++ b/result_test_full_features.xlsx
@@ -488,7 +488,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -590,7 +590,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -635,6 +635,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -649,9 +652,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -1028,7 +1028,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1556,156 +1556,182 @@
         <v/>
       </c>
     </row>
-    <row r="32" ht="30" customHeight="1">
-      <c r="A32" s="8" t="inlineStr">
+    <row r="32" ht="36" customHeight="1">
+      <c r="A32" s="15" t="inlineStr">
+        <is>
+          <t>NW(KGS)</t>
+        </is>
+      </c>
+      <c r="B32" s="16" t="n">
+        <v>14811.5001</v>
+      </c>
+      <c r="C32" s="16" t="n"/>
+      <c r="D32" s="16" t="n"/>
+      <c r="E32" s="16" t="n"/>
+    </row>
+    <row r="33" ht="36" customHeight="1">
+      <c r="A33" s="15" t="inlineStr">
+        <is>
+          <t>GW(KGS):</t>
+        </is>
+      </c>
+      <c r="B33" s="16" t="n">
+        <v>15711.5</v>
+      </c>
+      <c r="C33" s="16" t="n"/>
+      <c r="D33" s="16" t="n"/>
+      <c r="E33" s="16" t="n"/>
+    </row>
+    <row r="34" ht="30" customHeight="1">
+      <c r="A34" s="8" t="inlineStr">
         <is>
           <t>Term of Payment: 100% TT after shipment</t>
         </is>
       </c>
-      <c r="B32" s="8" t="n"/>
-      <c r="C32" s="8" t="n"/>
-      <c r="D32" s="8" t="n"/>
-      <c r="E32" s="8" t="n"/>
-      <c r="F32" s="2" t="n"/>
-    </row>
-    <row r="33" ht="36" customHeight="1">
-      <c r="A33" s="8" t="inlineStr">
-        <is>
-          <t>Transaction method: FCA(USD)</t>
-        </is>
-      </c>
-      <c r="B33" s="8" t="n"/>
-      <c r="C33" s="8" t="n"/>
-      <c r="D33" s="8" t="n"/>
-      <c r="E33" s="8" t="n"/>
-      <c r="F33" s="2" t="n"/>
-    </row>
-    <row r="34" ht="20.4" customHeight="1">
-      <c r="A34" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Beneficiary bank information: </t>
-        </is>
-      </c>
       <c r="B34" s="8" t="n"/>
-      <c r="C34" s="8" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
-        </is>
-      </c>
+      <c r="C34" s="8" t="n"/>
       <c r="D34" s="8" t="n"/>
       <c r="E34" s="8" t="n"/>
       <c r="F34" s="2" t="n"/>
     </row>
-    <row r="35" ht="45.9" customHeight="1">
+    <row r="35" ht="36" customHeight="1">
       <c r="A35" s="8" t="inlineStr">
         <is>
+          <t>Transaction method: DAF(USD)</t>
+        </is>
+      </c>
+      <c r="B35" s="8" t="n"/>
+      <c r="C35" s="8" t="n"/>
+      <c r="D35" s="8" t="n"/>
+      <c r="E35" s="8" t="n"/>
+      <c r="F35" s="2" t="n"/>
+    </row>
+    <row r="36" ht="20.4" customHeight="1">
+      <c r="A36" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beneficiary bank information: </t>
+        </is>
+      </c>
+      <c r="B36" s="8" t="n"/>
+      <c r="C36" s="8" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
+        </is>
+      </c>
+      <c r="D36" s="8" t="n"/>
+      <c r="E36" s="8" t="n"/>
+      <c r="F36" s="2" t="n"/>
+    </row>
+    <row r="37" ht="45.9" customHeight="1">
+      <c r="A37" s="8" t="inlineStr">
+        <is>
           <t xml:space="preserve">Beneficiary Bank' s Name: </t>
         </is>
       </c>
-      <c r="B35" s="8" t="n"/>
-      <c r="C35" s="14" t="inlineStr">
+      <c r="B37" s="8" t="n"/>
+      <c r="C37" s="14" t="inlineStr">
         <is>
           <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
  /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="F35" s="2" t="n"/>
-    </row>
-    <row r="36" ht="41.1" customHeight="1">
-      <c r="A36" s="8" t="inlineStr">
+      <c r="F37" s="2" t="n"/>
+    </row>
+    <row r="38" ht="41.1" customHeight="1">
+      <c r="A38" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">Bank Address:  </t>
         </is>
       </c>
-      <c r="B36" s="8" t="n"/>
-      <c r="C36" s="14" t="inlineStr">
+      <c r="B38" s="8" t="n"/>
+      <c r="C38" s="14" t="inlineStr">
         <is>
           <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.
 PHNOM PEMH,CAMBODIA.</t>
         </is>
       </c>
-      <c r="F36" s="2" t="n"/>
-    </row>
-    <row r="37" ht="29.1" customHeight="1">
-      <c r="A37" s="8" t="inlineStr">
+      <c r="F38" s="2" t="n"/>
+    </row>
+    <row r="39" ht="29.1" customHeight="1">
+      <c r="A39" s="8" t="inlineStr">
         <is>
           <t>Bank account :</t>
         </is>
       </c>
-      <c r="B37" s="8" t="n"/>
-      <c r="C37" s="19" t="inlineStr">
+      <c r="B39" s="8" t="n"/>
+      <c r="C39" s="19" t="inlineStr">
         <is>
           <t>100001100764430</t>
         </is>
       </c>
-      <c r="F37" s="2" t="n"/>
-    </row>
-    <row r="38" ht="19.2" customHeight="1">
-      <c r="A38" s="8" t="inlineStr">
+      <c r="F39" s="2" t="n"/>
+    </row>
+    <row r="40" ht="19.2" customHeight="1">
+      <c r="A40" s="8" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：</t>
         </is>
       </c>
-      <c r="B38" s="8" t="n"/>
-      <c r="C38" s="8" t="inlineStr">
+      <c r="B40" s="8" t="n"/>
+      <c r="C40" s="8" t="inlineStr">
         <is>
           <t>BKCHKHPPXXX</t>
         </is>
       </c>
-      <c r="D38" s="8" t="n"/>
-      <c r="E38" s="8" t="n"/>
-      <c r="F38" s="2" t="n"/>
-    </row>
-    <row r="39" ht="45.9" customHeight="1">
-      <c r="A39" s="8" t="n"/>
-      <c r="B39" s="8" t="n"/>
-      <c r="C39" s="8" t="n"/>
-      <c r="D39" s="8" t="n"/>
-      <c r="E39" s="8" t="n"/>
-      <c r="F39" s="8" t="n"/>
-    </row>
-    <row r="40" ht="41.1" customHeight="1">
-      <c r="A40" s="20" t="inlineStr">
+      <c r="D40" s="8" t="n"/>
+      <c r="E40" s="8" t="n"/>
+      <c r="F40" s="2" t="n"/>
+    </row>
+    <row r="41" ht="45.9" customHeight="1">
+      <c r="A41" s="8" t="n"/>
+      <c r="B41" s="8" t="n"/>
+      <c r="C41" s="8" t="n"/>
+      <c r="D41" s="8" t="n"/>
+      <c r="E41" s="8" t="n"/>
+      <c r="F41" s="8" t="n"/>
+    </row>
+    <row r="42" ht="41.1" customHeight="1">
+      <c r="A42" s="20" t="inlineStr">
         <is>
           <t>The Buyer:</t>
         </is>
       </c>
-      <c r="B40" s="2" t="n"/>
-      <c r="C40" s="2" t="n"/>
-      <c r="D40" s="21" t="inlineStr">
+      <c r="B42" s="2" t="n"/>
+      <c r="C42" s="2" t="n"/>
+      <c r="D42" s="21" t="inlineStr">
         <is>
           <t>The Seller:</t>
         </is>
       </c>
-      <c r="E40" s="2" t="n"/>
-      <c r="F40" s="2" t="n"/>
-    </row>
-    <row r="41" ht="29.1" customHeight="1">
-      <c r="A41" s="22" t="inlineStr">
+      <c r="E42" s="2" t="n"/>
+      <c r="F42" s="2" t="n"/>
+    </row>
+    <row r="43" ht="29.1" customHeight="1">
+      <c r="A43" s="22" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
       </c>
-      <c r="B41" s="23" t="n"/>
-      <c r="C41" s="24" t="n"/>
-      <c r="D41" s="22" t="inlineStr">
+      <c r="B43" s="23" t="n"/>
+      <c r="C43" s="24" t="n"/>
+      <c r="D43" s="22" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
         </is>
       </c>
-      <c r="E41" s="22" t="n"/>
-      <c r="F41" s="2" t="n"/>
+      <c r="E43" s="22" t="n"/>
+      <c r="F43" s="2" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C36:E36"/>
     <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C39:E39"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C38:E38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1717,7 +1743,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1940,12 +1966,12 @@
       <c r="E10" s="32" t="n"/>
       <c r="F10" s="40" t="inlineStr">
         <is>
-          <t>FCA :</t>
+          <t>DAF :</t>
         </is>
       </c>
       <c r="G10" s="41" t="inlineStr">
         <is>
-          <t>BAVET, SVAYRIENG</t>
+          <t>BAVET</t>
         </is>
       </c>
       <c r="H10" s="2" t="n"/>
@@ -2586,57 +2612,52 @@
         <v/>
       </c>
     </row>
-    <row r="39" ht="61.5" customHeight="1">
-      <c r="A39" s="64" t="inlineStr">
+    <row r="39" ht="35" customHeight="1">
+      <c r="A39" s="54" t="n"/>
+      <c r="B39" s="54" t="inlineStr">
+        <is>
+          <t>NW(KGS)</t>
+        </is>
+      </c>
+      <c r="C39" s="56" t="n">
+        <v>14811.5001</v>
+      </c>
+      <c r="D39" s="55" t="n"/>
+      <c r="E39" s="56" t="n"/>
+      <c r="F39" s="56" t="n"/>
+      <c r="G39" s="56" t="n"/>
+    </row>
+    <row r="40" ht="35" customHeight="1">
+      <c r="A40" s="54" t="n"/>
+      <c r="B40" s="54" t="inlineStr">
+        <is>
+          <t>GW(KGS):</t>
+        </is>
+      </c>
+      <c r="C40" s="56" t="n">
+        <v>15711.5</v>
+      </c>
+      <c r="D40" s="55" t="n"/>
+      <c r="E40" s="56" t="n"/>
+      <c r="F40" s="56" t="n"/>
+      <c r="G40" s="56" t="n"/>
+    </row>
+    <row r="41" ht="61.5" customHeight="1">
+      <c r="A41" s="64" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B39" s="65" t="inlineStr">
+      <c r="B41" s="65" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="D39" s="65" t="n"/>
-      <c r="E39" s="65" t="n"/>
-      <c r="F39" s="32" t="n"/>
-      <c r="G39" s="26" t="n"/>
-      <c r="H39" s="2" t="n"/>
-      <c r="I39" s="2" t="n"/>
-      <c r="J39" s="2" t="n"/>
-      <c r="K39" s="2" t="n"/>
-      <c r="L39" s="66" t="n"/>
-      <c r="M39" s="67" t="n"/>
-      <c r="N39" s="68" t="n"/>
-      <c r="O39" s="68" t="n"/>
-    </row>
-    <row r="40" ht="42" customHeight="1">
-      <c r="A40" s="69" t="inlineStr">
-        <is>
-          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
-                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-      <c r="D40" s="69" t="n"/>
-      <c r="E40" s="69" t="n"/>
-      <c r="F40" s="69" t="n"/>
-      <c r="G40" s="26" t="n"/>
-      <c r="H40" s="2" t="n"/>
-      <c r="I40" s="2" t="n"/>
-      <c r="J40" s="2" t="n"/>
-      <c r="K40" s="2" t="n"/>
-      <c r="L40" s="66" t="n"/>
-      <c r="M40" s="67" t="n"/>
-      <c r="N40" s="68" t="n"/>
-      <c r="O40" s="68" t="n"/>
-    </row>
-    <row r="41" ht="24.75" customHeight="1">
-      <c r="A41" s="70" t="inlineStr">
-        <is>
-          <t>A/C NO:100001100764430</t>
-        </is>
-      </c>
+      <c r="D41" s="65" t="n"/>
+      <c r="E41" s="65" t="n"/>
+      <c r="F41" s="32" t="n"/>
+      <c r="G41" s="26" t="n"/>
       <c r="H41" s="2" t="n"/>
       <c r="I41" s="2" t="n"/>
       <c r="J41" s="2" t="n"/>
@@ -2646,12 +2667,17 @@
       <c r="N41" s="68" t="n"/>
       <c r="O41" s="68" t="n"/>
     </row>
-    <row r="42" ht="27" customHeight="1">
-      <c r="A42" s="70" t="inlineStr">
-        <is>
-          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
-        </is>
-      </c>
+    <row r="42" ht="42" customHeight="1">
+      <c r="A42" s="69" t="inlineStr">
+        <is>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
+                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="D42" s="69" t="n"/>
+      <c r="E42" s="69" t="n"/>
+      <c r="F42" s="69" t="n"/>
+      <c r="G42" s="26" t="n"/>
       <c r="H42" s="2" t="n"/>
       <c r="I42" s="2" t="n"/>
       <c r="J42" s="2" t="n"/>
@@ -2661,19 +2687,13 @@
       <c r="N42" s="68" t="n"/>
       <c r="O42" s="68" t="n"/>
     </row>
-    <row r="43" ht="61.5" customHeight="1">
-      <c r="A43" s="2" t="n"/>
-      <c r="B43" s="2" t="n"/>
-      <c r="C43" s="2" t="n"/>
-      <c r="D43" s="2" t="n"/>
-      <c r="E43" s="71" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
-        </is>
-      </c>
-      <c r="F43" s="71" t="n"/>
-      <c r="G43" s="71" t="n"/>
-      <c r="H43" s="71" t="n"/>
+    <row r="43" ht="24.75" customHeight="1">
+      <c r="A43" s="70" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
+        </is>
+      </c>
+      <c r="H43" s="2" t="n"/>
       <c r="I43" s="2" t="n"/>
       <c r="J43" s="2" t="n"/>
       <c r="K43" s="2" t="n"/>
@@ -2682,18 +2702,12 @@
       <c r="N43" s="68" t="n"/>
       <c r="O43" s="68" t="n"/>
     </row>
-    <row r="44" ht="42" customHeight="1">
-      <c r="A44" s="2" t="n"/>
-      <c r="B44" s="2" t="n"/>
-      <c r="C44" s="2" t="n"/>
-      <c r="D44" s="72" t="n"/>
-      <c r="E44" s="73" t="n"/>
-      <c r="F44" s="74" t="inlineStr">
-        <is>
-          <t>Sign &amp; Stamp</t>
-        </is>
-      </c>
-      <c r="G44" s="75" t="n"/>
+    <row r="44" ht="27" customHeight="1">
+      <c r="A44" s="70" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
       <c r="H44" s="2" t="n"/>
       <c r="I44" s="2" t="n"/>
       <c r="J44" s="2" t="n"/>
@@ -2703,15 +2717,19 @@
       <c r="N44" s="68" t="n"/>
       <c r="O44" s="68" t="n"/>
     </row>
-    <row r="45" ht="24.75" customHeight="1">
+    <row r="45" ht="61.5" customHeight="1">
       <c r="A45" s="2" t="n"/>
       <c r="B45" s="2" t="n"/>
       <c r="C45" s="2" t="n"/>
-      <c r="D45" s="72" t="n"/>
-      <c r="E45" s="73" t="n"/>
-      <c r="F45" s="73" t="n"/>
-      <c r="G45" s="75" t="n"/>
-      <c r="H45" s="2" t="n"/>
+      <c r="D45" s="2" t="n"/>
+      <c r="E45" s="71" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="F45" s="71" t="n"/>
+      <c r="G45" s="71" t="n"/>
+      <c r="H45" s="71" t="n"/>
       <c r="I45" s="2" t="n"/>
       <c r="J45" s="2" t="n"/>
       <c r="K45" s="2" t="n"/>
@@ -2720,13 +2738,17 @@
       <c r="N45" s="68" t="n"/>
       <c r="O45" s="68" t="n"/>
     </row>
-    <row r="46" ht="27" customHeight="1">
+    <row r="46" ht="42" customHeight="1">
       <c r="A46" s="2" t="n"/>
       <c r="B46" s="2" t="n"/>
       <c r="C46" s="2" t="n"/>
       <c r="D46" s="72" t="n"/>
       <c r="E46" s="73" t="n"/>
-      <c r="F46" s="73" t="n"/>
+      <c r="F46" s="74" t="inlineStr">
+        <is>
+          <t>Sign &amp; Stamp</t>
+        </is>
+      </c>
       <c r="G46" s="75" t="n"/>
       <c r="H46" s="2" t="n"/>
       <c r="I46" s="2" t="n"/>
@@ -2737,18 +2759,14 @@
       <c r="N46" s="68" t="n"/>
       <c r="O46" s="68" t="n"/>
     </row>
-    <row r="47" ht="21" customHeight="1">
+    <row r="47" ht="24.75" customHeight="1">
       <c r="A47" s="2" t="n"/>
       <c r="B47" s="2" t="n"/>
       <c r="C47" s="2" t="n"/>
       <c r="D47" s="72" t="n"/>
       <c r="E47" s="73" t="n"/>
-      <c r="F47" s="76" t="inlineStr">
-        <is>
-          <t>ZENG XUELI</t>
-        </is>
-      </c>
-      <c r="G47" s="76" t="n"/>
+      <c r="F47" s="73" t="n"/>
+      <c r="G47" s="75" t="n"/>
       <c r="H47" s="2" t="n"/>
       <c r="I47" s="2" t="n"/>
       <c r="J47" s="2" t="n"/>
@@ -2758,18 +2776,56 @@
       <c r="N47" s="68" t="n"/>
       <c r="O47" s="68" t="n"/>
     </row>
+    <row r="48" ht="27" customHeight="1">
+      <c r="A48" s="2" t="n"/>
+      <c r="B48" s="2" t="n"/>
+      <c r="C48" s="2" t="n"/>
+      <c r="D48" s="72" t="n"/>
+      <c r="E48" s="73" t="n"/>
+      <c r="F48" s="73" t="n"/>
+      <c r="G48" s="75" t="n"/>
+      <c r="H48" s="2" t="n"/>
+      <c r="I48" s="2" t="n"/>
+      <c r="J48" s="2" t="n"/>
+      <c r="K48" s="2" t="n"/>
+      <c r="L48" s="66" t="n"/>
+      <c r="M48" s="67" t="n"/>
+      <c r="N48" s="68" t="n"/>
+      <c r="O48" s="68" t="n"/>
+    </row>
+    <row r="49" ht="21" customHeight="1">
+      <c r="A49" s="2" t="n"/>
+      <c r="B49" s="2" t="n"/>
+      <c r="C49" s="2" t="n"/>
+      <c r="D49" s="72" t="n"/>
+      <c r="E49" s="73" t="n"/>
+      <c r="F49" s="76" t="inlineStr">
+        <is>
+          <t>ZENG XUELI</t>
+        </is>
+      </c>
+      <c r="G49" s="76" t="n"/>
+      <c r="H49" s="2" t="n"/>
+      <c r="I49" s="2" t="n"/>
+      <c r="J49" s="2" t="n"/>
+      <c r="K49" s="2" t="n"/>
+      <c r="L49" s="66" t="n"/>
+      <c r="M49" s="67" t="n"/>
+      <c r="N49" s="68" t="n"/>
+      <c r="O49" s="68" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A44:G44"/>
     <mergeCell ref="D22:D36"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A43:G43"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2782,7 +2838,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T83"/>
+  <dimension ref="A1:T91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3052,12 +3108,12 @@
       <c r="G10" s="26" t="n"/>
       <c r="H10" s="40" t="inlineStr">
         <is>
-          <t>FCA :</t>
+          <t>DAF :</t>
         </is>
       </c>
       <c r="I10" s="81" t="inlineStr">
         <is>
-          <t>BAVET, SVAY RIENG</t>
+          <t>BAVET</t>
         </is>
       </c>
       <c r="J10" s="2" t="n"/>
@@ -4264,142 +4320,108 @@
         <v/>
       </c>
     </row>
+    <row r="55" ht="27" customHeight="1">
+      <c r="A55" s="55" t="n"/>
+      <c r="C55" s="55" t="inlineStr">
+        <is>
+          <t>NW(KGS)</t>
+        </is>
+      </c>
+      <c r="D55" s="100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="55" t="n"/>
+      <c r="F55" s="93" t="n"/>
+      <c r="G55" s="56" t="n"/>
+      <c r="H55" s="56" t="n"/>
+      <c r="I55" s="56" t="n"/>
+      <c r="J55" s="90" t="n"/>
+    </row>
     <row r="56" ht="27" customHeight="1">
-      <c r="A56" s="55" t="inlineStr">
+      <c r="A56" s="55" t="n"/>
+      <c r="C56" s="55" t="inlineStr">
+        <is>
+          <t>GW(KGS):</t>
+        </is>
+      </c>
+      <c r="D56" s="100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="55" t="n"/>
+      <c r="F56" s="93" t="n"/>
+      <c r="G56" s="56" t="n"/>
+      <c r="H56" s="56" t="n"/>
+      <c r="I56" s="56" t="n"/>
+      <c r="J56" s="90" t="n"/>
+    </row>
+    <row r="58" ht="27" customHeight="1">
+      <c r="A58" s="55" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B56" s="88" t="n"/>
-      <c r="C56" s="55" t="inlineStr">
+      <c r="B58" s="88" t="n"/>
+      <c r="C58" s="55" t="inlineStr">
         <is>
           <t>P.O Nº</t>
         </is>
       </c>
-      <c r="D56" s="55" t="inlineStr">
+      <c r="D58" s="55" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="E56" s="55" t="inlineStr">
+      <c r="E58" s="55" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F56" s="55" t="inlineStr">
+      <c r="F58" s="55" t="inlineStr">
         <is>
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="G56" s="89" t="n"/>
-      <c r="H56" s="56" t="inlineStr">
+      <c r="G58" s="89" t="n"/>
+      <c r="H58" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="I56" s="56" t="inlineStr">
+      <c r="I58" s="56" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="J56" s="90" t="inlineStr">
+      <c r="J58" s="90" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
-    <row r="57" ht="27" customHeight="1">
-      <c r="A57" s="91" t="n"/>
-      <c r="B57" s="92" t="n"/>
-      <c r="C57" s="62" t="n"/>
-      <c r="D57" s="62" t="n"/>
-      <c r="E57" s="62" t="n"/>
-      <c r="F57" s="93" t="inlineStr">
+    <row r="59" ht="27" customHeight="1">
+      <c r="A59" s="91" t="n"/>
+      <c r="B59" s="92" t="n"/>
+      <c r="C59" s="62" t="n"/>
+      <c r="D59" s="62" t="n"/>
+      <c r="E59" s="62" t="n"/>
+      <c r="F59" s="93" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="G57" s="56" t="inlineStr">
+      <c r="G59" s="56" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="H57" s="62" t="n"/>
-      <c r="I57" s="62" t="n"/>
-      <c r="J57" s="62" t="n"/>
-    </row>
-    <row r="58" ht="27" customHeight="1">
-      <c r="A58" s="94" t="inlineStr">
-        <is>
-          <t>VENDOR#:</t>
-        </is>
-      </c>
-      <c r="B58" s="95" t="n"/>
-      <c r="C58" s="96" t="n">
-        <v>9000701604</v>
-      </c>
-      <c r="D58" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E58" s="59" t="inlineStr">
-        <is>
-          <t>LEATHER</t>
-        </is>
-      </c>
-      <c r="F58" s="97" t="n">
-        <v>195</v>
-      </c>
-      <c r="G58" s="60" t="n">
-        <v>10187.1</v>
-      </c>
-      <c r="H58" s="60" t="n">
-        <v>842.5</v>
-      </c>
-      <c r="I58" s="60" t="n">
-        <v>887.5</v>
-      </c>
-      <c r="J58" s="98" t="n">
-        <v>2.6532</v>
-      </c>
-    </row>
-    <row r="59" ht="27" customHeight="1">
-      <c r="A59" s="94" t="inlineStr">
-        <is>
-          <t>Des: LEATHER</t>
-        </is>
-      </c>
-      <c r="B59" s="95" t="n"/>
-      <c r="C59" s="96" t="n">
-        <v>9000701604</v>
-      </c>
-      <c r="D59" s="96" t="inlineStr">
-        <is>
-          <t>01.10.U528073</t>
-        </is>
-      </c>
-      <c r="E59" s="61" t="n"/>
-      <c r="F59" s="97" t="n">
-        <v>195</v>
-      </c>
-      <c r="G59" s="60" t="n">
-        <v>10219.2</v>
-      </c>
-      <c r="H59" s="60" t="n">
-        <v>846</v>
-      </c>
-      <c r="I59" s="60" t="n">
-        <v>891</v>
-      </c>
-      <c r="J59" s="98" t="n">
-        <v>2.4948</v>
-      </c>
+      <c r="H59" s="62" t="n"/>
+      <c r="I59" s="62" t="n"/>
+      <c r="J59" s="62" t="n"/>
     </row>
     <row r="60" ht="27" customHeight="1">
       <c r="A60" s="94" t="inlineStr">
         <is>
-          <t>Case Qty:</t>
+          <t>VENDOR#:</t>
         </is>
       </c>
       <c r="B60" s="95" t="n"/>
@@ -4411,27 +4433,31 @@
           <t>01.10.U528073</t>
         </is>
       </c>
-      <c r="E60" s="61" t="n"/>
+      <c r="E60" s="59" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
       <c r="F60" s="97" t="n">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G60" s="60" t="n">
-        <v>10773.3</v>
+        <v>10187.1</v>
       </c>
       <c r="H60" s="60" t="n">
-        <v>883.7671</v>
+        <v>842.5</v>
       </c>
       <c r="I60" s="60" t="n">
-        <v>926.3013999999999</v>
+        <v>887.5</v>
       </c>
       <c r="J60" s="98" t="n">
-        <v>2.8447</v>
+        <v>2.6532</v>
       </c>
     </row>
     <row r="61" ht="27" customHeight="1">
       <c r="A61" s="94" t="inlineStr">
         <is>
-          <t>MADE IN CAMBODIA</t>
+          <t>Des: LEATHER</t>
         </is>
       </c>
       <c r="B61" s="95" t="n"/>
@@ -4445,22 +4471,28 @@
       </c>
       <c r="E61" s="61" t="n"/>
       <c r="F61" s="97" t="n">
-        <v>12</v>
+        <v>195</v>
       </c>
       <c r="G61" s="60" t="n">
-        <v>479.1</v>
+        <v>10219.2</v>
       </c>
       <c r="H61" s="60" t="n">
-        <v>51.2329</v>
+        <v>846</v>
       </c>
       <c r="I61" s="60" t="n">
-        <v>53.6986</v>
+        <v>891</v>
       </c>
       <c r="J61" s="98" t="n">
-        <v>0.1649</v>
+        <v>2.4948</v>
       </c>
     </row>
     <row r="62" ht="27" customHeight="1">
+      <c r="A62" s="94" t="inlineStr">
+        <is>
+          <t>Case Qty:</t>
+        </is>
+      </c>
+      <c r="B62" s="95" t="n"/>
       <c r="C62" s="96" t="n">
         <v>9000701604</v>
       </c>
@@ -4471,22 +4503,28 @@
       </c>
       <c r="E62" s="61" t="n"/>
       <c r="F62" s="97" t="n">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="G62" s="60" t="n">
-        <v>10215.8</v>
+        <v>10773.3</v>
       </c>
       <c r="H62" s="60" t="n">
-        <v>840</v>
+        <v>883.7671</v>
       </c>
       <c r="I62" s="60" t="n">
-        <v>885</v>
+        <v>926.3013999999999</v>
       </c>
       <c r="J62" s="98" t="n">
-        <v>2.6136</v>
+        <v>2.8447</v>
       </c>
     </row>
     <row r="63" ht="27" customHeight="1">
+      <c r="A63" s="94" t="inlineStr">
+        <is>
+          <t>MADE IN CAMBODIA</t>
+        </is>
+      </c>
+      <c r="B63" s="95" t="n"/>
       <c r="C63" s="96" t="n">
         <v>9000701604</v>
       </c>
@@ -4497,19 +4535,19 @@
       </c>
       <c r="E63" s="61" t="n"/>
       <c r="F63" s="97" t="n">
-        <v>195</v>
+        <v>12</v>
       </c>
       <c r="G63" s="60" t="n">
-        <v>10237.5</v>
+        <v>479.1</v>
       </c>
       <c r="H63" s="60" t="n">
-        <v>863.5</v>
+        <v>51.2329</v>
       </c>
       <c r="I63" s="60" t="n">
-        <v>908.5</v>
+        <v>53.6986</v>
       </c>
       <c r="J63" s="98" t="n">
-        <v>2.6928</v>
+        <v>0.1649</v>
       </c>
     </row>
     <row r="64" ht="27" customHeight="1">
@@ -4526,13 +4564,13 @@
         <v>195</v>
       </c>
       <c r="G64" s="60" t="n">
-        <v>10196.1</v>
+        <v>10215.8</v>
       </c>
       <c r="H64" s="60" t="n">
-        <v>849</v>
+        <v>840</v>
       </c>
       <c r="I64" s="60" t="n">
-        <v>894</v>
+        <v>885</v>
       </c>
       <c r="J64" s="98" t="n">
         <v>2.6136</v>
@@ -4549,19 +4587,19 @@
       </c>
       <c r="E65" s="61" t="n"/>
       <c r="F65" s="97" t="n">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="G65" s="60" t="n">
-        <v>9097.6</v>
+        <v>10237.5</v>
       </c>
       <c r="H65" s="60" t="n">
-        <v>739.443</v>
+        <v>863.5</v>
       </c>
       <c r="I65" s="60" t="n">
-        <v>780.2461</v>
+        <v>908.5</v>
       </c>
       <c r="J65" s="98" t="n">
-        <v>2.3339</v>
+        <v>2.6928</v>
       </c>
     </row>
     <row r="66" ht="27" customHeight="1">
@@ -4575,19 +4613,19 @@
       </c>
       <c r="E66" s="61" t="n"/>
       <c r="F66" s="97" t="n">
-        <v>18</v>
+        <v>195</v>
       </c>
       <c r="G66" s="60" t="n">
-        <v>726</v>
+        <v>10196.1</v>
       </c>
       <c r="H66" s="60" t="n">
-        <v>76.057</v>
+        <v>849</v>
       </c>
       <c r="I66" s="60" t="n">
-        <v>80.2539</v>
+        <v>894</v>
       </c>
       <c r="J66" s="98" t="n">
-        <v>0.2401</v>
+        <v>2.6136</v>
       </c>
     </row>
     <row r="67" ht="27" customHeight="1">
@@ -4601,19 +4639,19 @@
       </c>
       <c r="E67" s="61" t="n"/>
       <c r="F67" s="97" t="n">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="G67" s="60" t="n">
-        <v>10110.4</v>
+        <v>9097.6</v>
       </c>
       <c r="H67" s="60" t="n">
-        <v>840</v>
+        <v>739.443</v>
       </c>
       <c r="I67" s="60" t="n">
-        <v>885</v>
+        <v>780.2461</v>
       </c>
       <c r="J67" s="98" t="n">
-        <v>2.574</v>
+        <v>2.3339</v>
       </c>
     </row>
     <row r="68" ht="27" customHeight="1">
@@ -4627,19 +4665,19 @@
       </c>
       <c r="E68" s="61" t="n"/>
       <c r="F68" s="97" t="n">
-        <v>195</v>
+        <v>18</v>
       </c>
       <c r="G68" s="60" t="n">
-        <v>10165.7</v>
+        <v>726</v>
       </c>
       <c r="H68" s="60" t="n">
-        <v>844.5</v>
+        <v>76.057</v>
       </c>
       <c r="I68" s="60" t="n">
-        <v>889.5</v>
+        <v>80.2539</v>
       </c>
       <c r="J68" s="98" t="n">
-        <v>2.772</v>
+        <v>0.2401</v>
       </c>
     </row>
     <row r="69" ht="27" customHeight="1">
@@ -4656,368 +4694,331 @@
         <v>195</v>
       </c>
       <c r="G69" s="60" t="n">
-        <v>10222.1</v>
+        <v>10110.4</v>
       </c>
       <c r="H69" s="60" t="n">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="I69" s="60" t="n">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="J69" s="98" t="n">
-        <v>2.6136</v>
+        <v>2.574</v>
       </c>
     </row>
     <row r="70" ht="27" customHeight="1">
-      <c r="C70" s="96" t="inlineStr">
-        <is>
-          <t>9000678672</t>
-        </is>
+      <c r="C70" s="96" t="n">
+        <v>9000701604</v>
       </c>
       <c r="D70" s="96" t="inlineStr">
         <is>
-          <t>01.10.L2924</t>
+          <t>01.10.U528073</t>
         </is>
       </c>
       <c r="E70" s="61" t="n"/>
       <c r="F70" s="97" t="n">
+        <v>195</v>
+      </c>
+      <c r="G70" s="60" t="n">
+        <v>10165.7</v>
+      </c>
+      <c r="H70" s="60" t="n">
+        <v>844.5</v>
+      </c>
+      <c r="I70" s="60" t="n">
+        <v>889.5</v>
+      </c>
+      <c r="J70" s="98" t="n">
+        <v>2.772</v>
+      </c>
+    </row>
+    <row r="71" ht="27" customHeight="1">
+      <c r="C71" s="96" t="n">
+        <v>9000701604</v>
+      </c>
+      <c r="D71" s="96" t="inlineStr">
+        <is>
+          <t>01.10.U528073</t>
+        </is>
+      </c>
+      <c r="E71" s="61" t="n"/>
+      <c r="F71" s="97" t="n">
+        <v>195</v>
+      </c>
+      <c r="G71" s="60" t="n">
+        <v>10222.1</v>
+      </c>
+      <c r="H71" s="60" t="n">
+        <v>843</v>
+      </c>
+      <c r="I71" s="60" t="n">
+        <v>888</v>
+      </c>
+      <c r="J71" s="98" t="n">
+        <v>2.6136</v>
+      </c>
+    </row>
+    <row r="72" ht="27" customHeight="1">
+      <c r="C72" s="96" t="inlineStr">
+        <is>
+          <t>9000678672</t>
+        </is>
+      </c>
+      <c r="D72" s="96" t="inlineStr">
+        <is>
+          <t>01.10.L2924</t>
+        </is>
+      </c>
+      <c r="E72" s="61" t="n"/>
+      <c r="F72" s="97" t="n">
         <v>106</v>
       </c>
-      <c r="G70" s="60" t="n">
+      <c r="G72" s="60" t="n">
         <v>5345</v>
       </c>
-      <c r="H70" s="60" t="n">
+      <c r="H72" s="60" t="n">
         <v>381.211</v>
       </c>
-      <c r="I70" s="60" t="n">
+      <c r="I72" s="60" t="n">
         <v>424.9725</v>
       </c>
-      <c r="J70" s="98" t="n">
+      <c r="J72" s="98" t="n">
         <v>2.0795</v>
       </c>
     </row>
-    <row r="71" ht="27" customHeight="1">
-      <c r="C71" s="96" t="inlineStr">
+    <row r="73" ht="27" customHeight="1">
+      <c r="C73" s="96" t="inlineStr">
         <is>
           <t>9000678672</t>
         </is>
       </c>
-      <c r="D71" s="96" t="inlineStr">
+      <c r="D73" s="96" t="inlineStr">
         <is>
           <t>01.10.L2924</t>
         </is>
       </c>
-      <c r="E71" s="62" t="n"/>
-      <c r="F71" s="97" t="n">
+      <c r="E73" s="62" t="n"/>
+      <c r="F73" s="97" t="n">
         <v>3</v>
       </c>
-      <c r="G71" s="60" t="n">
+      <c r="G73" s="60" t="n">
         <v>121</v>
       </c>
-      <c r="H71" s="60" t="n">
+      <c r="H73" s="60" t="n">
         <v>10.789</v>
       </c>
-      <c r="I71" s="60" t="n">
+      <c r="I73" s="60" t="n">
         <v>12.0275</v>
       </c>
-      <c r="J71" s="98" t="n">
+      <c r="J73" s="98" t="n">
         <v>0.0589</v>
       </c>
     </row>
-    <row r="72" ht="27" customHeight="1">
-      <c r="A72" s="99" t="n"/>
-      <c r="C72" s="55" t="inlineStr">
+    <row r="74" ht="27" customHeight="1">
+      <c r="A74" s="99" t="n"/>
+      <c r="C74" s="55" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
         </is>
       </c>
-      <c r="D72" s="55" t="n"/>
-      <c r="E72" s="55" t="n"/>
-      <c r="F72" s="93" t="n"/>
-      <c r="G72" s="56" t="n"/>
-      <c r="H72" s="56" t="n"/>
-      <c r="I72" s="56" t="n"/>
-      <c r="J72" s="90" t="n"/>
-    </row>
-    <row r="73" ht="27" customHeight="1">
-      <c r="A73" s="55" t="n"/>
-      <c r="B73" s="89" t="n"/>
-      <c r="C73" s="55" t="inlineStr">
+      <c r="D74" s="55" t="n"/>
+      <c r="E74" s="55" t="n"/>
+      <c r="F74" s="93" t="n"/>
+      <c r="G74" s="56" t="n"/>
+      <c r="H74" s="56" t="n"/>
+      <c r="I74" s="56" t="n"/>
+      <c r="J74" s="90" t="n"/>
+    </row>
+    <row r="75" ht="27" customHeight="1">
+      <c r="A75" s="55" t="n"/>
+      <c r="B75" s="89" t="n"/>
+      <c r="C75" s="55" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="D73" s="55" t="inlineStr">
+      <c r="D75" s="55" t="inlineStr">
         <is>
           <t>11 PALLETS</t>
         </is>
       </c>
-      <c r="E73" s="55" t="n"/>
-      <c r="F73" s="93">
-        <f>SUM(F58:F71)</f>
+      <c r="E75" s="55" t="n"/>
+      <c r="F75" s="93">
+        <f>SUM(F60:F73)</f>
         <v/>
       </c>
-      <c r="G73" s="56">
-        <f>SUM(G58:G71)</f>
+      <c r="G75" s="56">
+        <f>SUM(G60:G73)</f>
         <v/>
       </c>
-      <c r="H73" s="56">
-        <f>SUM(H58:H71)</f>
+      <c r="H75" s="56">
+        <f>SUM(H60:H73)</f>
         <v/>
       </c>
-      <c r="I73" s="56">
-        <f>SUM(I58:I71)</f>
+      <c r="I75" s="56">
+        <f>SUM(I60:I73)</f>
         <v/>
       </c>
-      <c r="J73" s="90">
-        <f>SUM(J58:J71)</f>
+      <c r="J75" s="90">
+        <f>SUM(J60:J73)</f>
         <v/>
       </c>
     </row>
-    <row r="74" ht="27" customHeight="1">
-      <c r="A74" s="100" t="n"/>
-      <c r="C74" s="100" t="inlineStr">
+    <row r="76" ht="27" customHeight="1">
+      <c r="A76" s="55" t="n"/>
+      <c r="C76" s="55" t="inlineStr">
+        <is>
+          <t>NW(KGS)</t>
+        </is>
+      </c>
+      <c r="D76" s="100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" s="55" t="n"/>
+      <c r="F76" s="93" t="n"/>
+      <c r="G76" s="56" t="n"/>
+      <c r="H76" s="56" t="n"/>
+      <c r="I76" s="56" t="n"/>
+      <c r="J76" s="90" t="n"/>
+    </row>
+    <row r="77" ht="27" customHeight="1">
+      <c r="A77" s="55" t="n"/>
+      <c r="C77" s="55" t="inlineStr">
+        <is>
+          <t>GW(KGS):</t>
+        </is>
+      </c>
+      <c r="D77" s="100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" s="55" t="n"/>
+      <c r="F77" s="93" t="n"/>
+      <c r="G77" s="56" t="n"/>
+      <c r="H77" s="56" t="n"/>
+      <c r="I77" s="56" t="n"/>
+      <c r="J77" s="90" t="n"/>
+    </row>
+    <row r="78" ht="27" customHeight="1">
+      <c r="A78" s="101" t="n"/>
+      <c r="C78" s="101" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
         </is>
       </c>
-      <c r="D74" s="100" t="inlineStr">
+      <c r="D78" s="101" t="inlineStr">
         <is>
           <t>31 PALLETS</t>
         </is>
       </c>
-      <c r="E74" s="100" t="n"/>
-      <c r="F74" s="101">
-        <f>SUM(F23:F52,F58:F71)</f>
+      <c r="E78" s="101" t="n"/>
+      <c r="F78" s="102">
+        <f>SUM(F23:F52,F60:F73)</f>
         <v/>
       </c>
-      <c r="G74" s="102">
-        <f>SUM(G23:G52,G58:G71)</f>
+      <c r="G78" s="103">
+        <f>SUM(G23:G52,G60:G73)</f>
         <v/>
       </c>
-      <c r="H74" s="102">
-        <f>SUM(H23:H52,H58:H71)</f>
+      <c r="H78" s="103">
+        <f>SUM(H23:H52,H60:H73)</f>
         <v/>
       </c>
-      <c r="I74" s="102">
-        <f>SUM(I23:I52,I58:I71)</f>
+      <c r="I78" s="103">
+        <f>SUM(I23:I52,I60:I73)</f>
         <v/>
       </c>
-      <c r="J74" s="103">
-        <f>SUM(J23:J52,J58:J71)</f>
+      <c r="J78" s="104">
+        <f>SUM(J23:J52,J60:J73)</f>
         <v/>
       </c>
     </row>
-    <row r="75" ht="27" customHeight="1">
-      <c r="A75" s="2" t="n"/>
-      <c r="B75" s="2" t="n"/>
-      <c r="C75" s="2" t="n"/>
-      <c r="D75" s="2" t="n"/>
-      <c r="E75" s="2" t="n"/>
-      <c r="F75" s="2" t="n"/>
-      <c r="G75" s="2" t="n"/>
-      <c r="H75" s="2" t="n"/>
-      <c r="I75" s="2" t="n"/>
-      <c r="J75" s="2" t="n"/>
-      <c r="K75" s="2" t="n"/>
-      <c r="L75" s="2" t="n"/>
-      <c r="M75" s="2" t="n"/>
-      <c r="N75" s="2" t="n"/>
-      <c r="O75" s="2" t="n"/>
-      <c r="P75" s="2" t="n"/>
-      <c r="Q75" s="2" t="n"/>
-      <c r="R75" s="2" t="n"/>
-      <c r="S75" s="2" t="n"/>
-      <c r="T75" s="2" t="n"/>
-    </row>
-    <row r="76" ht="27" customHeight="1">
-      <c r="A76" s="2" t="n"/>
-      <c r="B76" s="2" t="n"/>
-      <c r="C76" s="2" t="n"/>
-      <c r="D76" s="2" t="n"/>
-      <c r="E76" s="2" t="n"/>
-      <c r="F76" s="2" t="n"/>
-      <c r="G76" s="2" t="n"/>
-      <c r="H76" s="2" t="n"/>
-      <c r="I76" s="2" t="n"/>
-      <c r="J76" s="2" t="n"/>
-      <c r="K76" s="2" t="n"/>
-      <c r="L76" s="2" t="n"/>
-      <c r="M76" s="2" t="n"/>
-      <c r="N76" s="2" t="n"/>
-      <c r="O76" s="2" t="n"/>
-      <c r="P76" s="2" t="n"/>
-      <c r="Q76" s="2" t="n"/>
-      <c r="R76" s="2" t="n"/>
-      <c r="S76" s="2" t="n"/>
-      <c r="T76" s="2" t="n"/>
-    </row>
-    <row r="77" ht="27" customHeight="1">
-      <c r="A77" s="53" t="n"/>
-      <c r="B77" s="87" t="n"/>
-      <c r="C77" s="2" t="n"/>
-      <c r="D77" s="2" t="n"/>
-      <c r="E77" s="2" t="n"/>
-      <c r="F77" s="2" t="n"/>
-      <c r="G77" s="2" t="n"/>
-      <c r="H77" s="2" t="n"/>
-      <c r="I77" s="2" t="n"/>
-      <c r="J77" s="2" t="n"/>
-      <c r="K77" s="2" t="n"/>
-      <c r="L77" s="2" t="n"/>
-      <c r="M77" s="2" t="n"/>
-      <c r="N77" s="2" t="n"/>
-      <c r="O77" s="2" t="n"/>
-      <c r="P77" s="2" t="n"/>
-      <c r="Q77" s="2" t="n"/>
-      <c r="R77" s="2" t="n"/>
-      <c r="S77" s="2" t="n"/>
-      <c r="T77" s="2" t="n"/>
-    </row>
-    <row r="78" ht="27" customHeight="1">
-      <c r="A78" s="104" t="inlineStr">
-        <is>
-          <t>Country of Original Cambodia</t>
-        </is>
-      </c>
-      <c r="B78" s="104" t="n"/>
-      <c r="C78" s="104" t="n"/>
-      <c r="D78" s="105" t="n"/>
-      <c r="E78" s="106" t="n"/>
-      <c r="F78" s="26" t="n"/>
-      <c r="G78" s="26" t="n"/>
-      <c r="H78" s="26" t="n"/>
-      <c r="I78" s="2" t="n"/>
-      <c r="J78" s="2" t="n"/>
-      <c r="K78" s="2" t="n"/>
-      <c r="L78" s="2" t="n"/>
-      <c r="M78" s="2" t="n"/>
-      <c r="N78" s="2" t="n"/>
-      <c r="O78" s="2" t="n"/>
-      <c r="P78" s="2" t="n"/>
-      <c r="Q78" s="2" t="n"/>
-      <c r="R78" s="2" t="n"/>
-      <c r="S78" s="2" t="n"/>
-      <c r="T78" s="2" t="n"/>
-    </row>
-    <row r="79" ht="65.25" customHeight="1">
-      <c r="A79" s="64" t="inlineStr">
-        <is>
-          <t>Manufacture:</t>
-        </is>
-      </c>
-      <c r="B79" s="107" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
-XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
-        </is>
-      </c>
-      <c r="E79" s="108" t="n"/>
-      <c r="F79" s="108" t="n"/>
-      <c r="G79" s="108" t="n"/>
-      <c r="H79" s="26" t="n"/>
-      <c r="I79" s="2" t="n"/>
-      <c r="J79" s="2" t="n"/>
-      <c r="K79" s="2" t="n"/>
-      <c r="L79" s="2" t="n"/>
-      <c r="M79" s="2" t="n"/>
-      <c r="N79" s="2" t="n"/>
-      <c r="O79" s="2" t="n"/>
-      <c r="P79" s="2" t="n"/>
-      <c r="Q79" s="2" t="n"/>
-      <c r="R79" s="2" t="n"/>
-      <c r="S79" s="2" t="n"/>
-      <c r="T79" s="2" t="n"/>
-    </row>
-    <row r="80" ht="51.75" customHeight="1">
-      <c r="A80" s="107" t="inlineStr">
-        <is>
-          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
-                                          /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-      <c r="E80" s="108" t="n"/>
-      <c r="F80" s="108" t="n"/>
-      <c r="G80" s="108" t="n"/>
-      <c r="H80" s="108" t="n"/>
-      <c r="I80" s="2" t="n"/>
-      <c r="J80" s="2" t="n"/>
-      <c r="K80" s="2" t="n"/>
-      <c r="L80" s="2" t="n"/>
-      <c r="M80" s="2" t="n"/>
-      <c r="N80" s="2" t="n"/>
-      <c r="O80" s="2" t="n"/>
-      <c r="P80" s="2" t="n"/>
-      <c r="Q80" s="2" t="n"/>
-      <c r="R80" s="2" t="n"/>
-      <c r="S80" s="2" t="n"/>
-      <c r="T80" s="2" t="n"/>
-    </row>
-    <row r="81" ht="27" customHeight="1">
-      <c r="A81" s="70" t="inlineStr">
-        <is>
-          <t>A/C NO:100001100764430</t>
-        </is>
-      </c>
-      <c r="B81" s="70" t="n"/>
-      <c r="C81" s="70" t="n"/>
-      <c r="D81" s="70" t="n"/>
-      <c r="E81" s="50" t="n"/>
-      <c r="F81" s="50" t="n"/>
-      <c r="G81" s="50" t="n"/>
-      <c r="H81" s="50" t="n"/>
-      <c r="I81" s="2" t="n"/>
-      <c r="J81" s="2" t="n"/>
-      <c r="K81" s="2" t="n"/>
-      <c r="L81" s="2" t="n"/>
-      <c r="M81" s="2" t="n"/>
-      <c r="N81" s="2" t="n"/>
-      <c r="O81" s="2" t="n"/>
-      <c r="P81" s="2" t="n"/>
-      <c r="Q81" s="2" t="n"/>
-      <c r="R81" s="2" t="n"/>
-      <c r="S81" s="2" t="n"/>
-      <c r="T81" s="2" t="n"/>
-    </row>
-    <row r="82" ht="27" customHeight="1">
-      <c r="A82" s="70" t="inlineStr">
-        <is>
-          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
-        </is>
-      </c>
-      <c r="B82" s="70" t="n"/>
-      <c r="C82" s="70" t="n"/>
-      <c r="D82" s="70" t="n"/>
-      <c r="E82" s="50" t="n"/>
-      <c r="F82" s="50" t="n"/>
-      <c r="G82" s="50" t="n"/>
-      <c r="H82" s="50" t="n"/>
-      <c r="I82" s="2" t="n"/>
-      <c r="J82" s="2" t="n"/>
-      <c r="K82" s="2" t="n"/>
-      <c r="L82" s="2" t="n"/>
-      <c r="M82" s="2" t="n"/>
-      <c r="N82" s="2" t="n"/>
-      <c r="O82" s="2" t="n"/>
-      <c r="P82" s="2" t="n"/>
-      <c r="Q82" s="2" t="n"/>
-      <c r="R82" s="2" t="n"/>
-      <c r="S82" s="2" t="n"/>
-      <c r="T82" s="2" t="n"/>
+    <row r="79" ht="27" customHeight="1">
+      <c r="A79" s="55" t="n"/>
+      <c r="C79" s="55" t="inlineStr">
+        <is>
+          <t>NW(KGS)</t>
+        </is>
+      </c>
+      <c r="D79" s="100" t="n">
+        <v>23722.5001</v>
+      </c>
+      <c r="E79" s="55" t="n"/>
+      <c r="F79" s="93" t="n"/>
+      <c r="G79" s="56" t="n"/>
+      <c r="H79" s="56" t="n"/>
+      <c r="I79" s="56" t="n"/>
+      <c r="J79" s="90" t="n"/>
+    </row>
+    <row r="80" ht="27" customHeight="1">
+      <c r="A80" s="55" t="n"/>
+      <c r="C80" s="55" t="inlineStr">
+        <is>
+          <t>GW(KGS):</t>
+        </is>
+      </c>
+      <c r="D80" s="100" t="n">
+        <v>25117.5</v>
+      </c>
+      <c r="E80" s="55" t="n"/>
+      <c r="F80" s="93" t="n"/>
+      <c r="G80" s="56" t="n"/>
+      <c r="H80" s="56" t="n"/>
+      <c r="I80" s="56" t="n"/>
+      <c r="J80" s="90" t="n"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="101" t="n"/>
+      <c r="C81" s="101" t="inlineStr">
+        <is>
+          <t>TOTAL OF BUFFALO LEATHER</t>
+        </is>
+      </c>
+      <c r="D81" s="101" t="n"/>
+      <c r="E81" s="101" t="n"/>
+      <c r="F81" s="102" t="n"/>
+      <c r="G81" s="103" t="n"/>
+      <c r="H81" s="103" t="n"/>
+      <c r="I81" s="103" t="n"/>
+      <c r="J81" s="104" t="n"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="101" t="n"/>
+      <c r="C82" s="101" t="inlineStr">
+        <is>
+          <t>TOTAL OF COW LEATHER</t>
+        </is>
+      </c>
+      <c r="D82" s="101" t="inlineStr">
+        <is>
+          <t>31 PALLETS</t>
+        </is>
+      </c>
+      <c r="E82" s="101" t="n"/>
+      <c r="F82" s="102" t="n">
+        <v>5662</v>
+      </c>
+      <c r="G82" s="103" t="n">
+        <v>293113.7</v>
+      </c>
+      <c r="H82" s="103" t="n">
+        <v>23722.5001</v>
+      </c>
+      <c r="I82" s="103" t="n">
+        <v>25117.5</v>
+      </c>
+      <c r="J82" s="104" t="n">
+        <v>76.86359999999999</v>
+      </c>
     </row>
     <row r="83" ht="27" customHeight="1">
       <c r="A83" s="2" t="n"/>
-      <c r="B83" s="109" t="n"/>
+      <c r="B83" s="2" t="n"/>
       <c r="C83" s="2" t="n"/>
       <c r="D83" s="2" t="n"/>
-      <c r="E83" s="52" t="n"/>
+      <c r="E83" s="2" t="n"/>
       <c r="F83" s="2" t="n"/>
-      <c r="G83" s="26" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
-        </is>
-      </c>
-      <c r="H83" s="52" t="n"/>
+      <c r="G83" s="2" t="n"/>
+      <c r="H83" s="2" t="n"/>
       <c r="I83" s="2" t="n"/>
       <c r="J83" s="2" t="n"/>
       <c r="K83" s="2" t="n"/>
@@ -5030,6 +5031,207 @@
       <c r="R83" s="2" t="n"/>
       <c r="S83" s="2" t="n"/>
       <c r="T83" s="2" t="n"/>
+    </row>
+    <row r="84" ht="27" customHeight="1">
+      <c r="A84" s="2" t="n"/>
+      <c r="B84" s="2" t="n"/>
+      <c r="C84" s="2" t="n"/>
+      <c r="D84" s="2" t="n"/>
+      <c r="E84" s="2" t="n"/>
+      <c r="F84" s="2" t="n"/>
+      <c r="G84" s="2" t="n"/>
+      <c r="H84" s="2" t="n"/>
+      <c r="I84" s="2" t="n"/>
+      <c r="J84" s="2" t="n"/>
+      <c r="K84" s="2" t="n"/>
+      <c r="L84" s="2" t="n"/>
+      <c r="M84" s="2" t="n"/>
+      <c r="N84" s="2" t="n"/>
+      <c r="O84" s="2" t="n"/>
+      <c r="P84" s="2" t="n"/>
+      <c r="Q84" s="2" t="n"/>
+      <c r="R84" s="2" t="n"/>
+      <c r="S84" s="2" t="n"/>
+      <c r="T84" s="2" t="n"/>
+    </row>
+    <row r="85" ht="27" customHeight="1">
+      <c r="A85" s="53" t="n"/>
+      <c r="B85" s="87" t="n"/>
+      <c r="C85" s="2" t="n"/>
+      <c r="D85" s="2" t="n"/>
+      <c r="E85" s="2" t="n"/>
+      <c r="F85" s="2" t="n"/>
+      <c r="G85" s="2" t="n"/>
+      <c r="H85" s="2" t="n"/>
+      <c r="I85" s="2" t="n"/>
+      <c r="J85" s="2" t="n"/>
+      <c r="K85" s="2" t="n"/>
+      <c r="L85" s="2" t="n"/>
+      <c r="M85" s="2" t="n"/>
+      <c r="N85" s="2" t="n"/>
+      <c r="O85" s="2" t="n"/>
+      <c r="P85" s="2" t="n"/>
+      <c r="Q85" s="2" t="n"/>
+      <c r="R85" s="2" t="n"/>
+      <c r="S85" s="2" t="n"/>
+      <c r="T85" s="2" t="n"/>
+    </row>
+    <row r="86" ht="27" customHeight="1">
+      <c r="A86" s="105" t="inlineStr">
+        <is>
+          <t>Country of Original Cambodia</t>
+        </is>
+      </c>
+      <c r="B86" s="105" t="n"/>
+      <c r="C86" s="105" t="n"/>
+      <c r="D86" s="41" t="n"/>
+      <c r="E86" s="106" t="n"/>
+      <c r="F86" s="26" t="n"/>
+      <c r="G86" s="26" t="n"/>
+      <c r="H86" s="26" t="n"/>
+      <c r="I86" s="2" t="n"/>
+      <c r="J86" s="2" t="n"/>
+      <c r="K86" s="2" t="n"/>
+      <c r="L86" s="2" t="n"/>
+      <c r="M86" s="2" t="n"/>
+      <c r="N86" s="2" t="n"/>
+      <c r="O86" s="2" t="n"/>
+      <c r="P86" s="2" t="n"/>
+      <c r="Q86" s="2" t="n"/>
+      <c r="R86" s="2" t="n"/>
+      <c r="S86" s="2" t="n"/>
+      <c r="T86" s="2" t="n"/>
+    </row>
+    <row r="87" ht="65.25" customHeight="1">
+      <c r="A87" s="64" t="inlineStr">
+        <is>
+          <t>Manufacture:</t>
+        </is>
+      </c>
+      <c r="B87" s="107" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
+XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="E87" s="108" t="n"/>
+      <c r="F87" s="108" t="n"/>
+      <c r="G87" s="108" t="n"/>
+      <c r="H87" s="26" t="n"/>
+      <c r="I87" s="2" t="n"/>
+      <c r="J87" s="2" t="n"/>
+      <c r="K87" s="2" t="n"/>
+      <c r="L87" s="2" t="n"/>
+      <c r="M87" s="2" t="n"/>
+      <c r="N87" s="2" t="n"/>
+      <c r="O87" s="2" t="n"/>
+      <c r="P87" s="2" t="n"/>
+      <c r="Q87" s="2" t="n"/>
+      <c r="R87" s="2" t="n"/>
+      <c r="S87" s="2" t="n"/>
+      <c r="T87" s="2" t="n"/>
+    </row>
+    <row r="88" ht="51.75" customHeight="1">
+      <c r="A88" s="107" t="inlineStr">
+        <is>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
+                                          /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="E88" s="108" t="n"/>
+      <c r="F88" s="108" t="n"/>
+      <c r="G88" s="108" t="n"/>
+      <c r="H88" s="108" t="n"/>
+      <c r="I88" s="2" t="n"/>
+      <c r="J88" s="2" t="n"/>
+      <c r="K88" s="2" t="n"/>
+      <c r="L88" s="2" t="n"/>
+      <c r="M88" s="2" t="n"/>
+      <c r="N88" s="2" t="n"/>
+      <c r="O88" s="2" t="n"/>
+      <c r="P88" s="2" t="n"/>
+      <c r="Q88" s="2" t="n"/>
+      <c r="R88" s="2" t="n"/>
+      <c r="S88" s="2" t="n"/>
+      <c r="T88" s="2" t="n"/>
+    </row>
+    <row r="89" ht="27" customHeight="1">
+      <c r="A89" s="70" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
+        </is>
+      </c>
+      <c r="B89" s="70" t="n"/>
+      <c r="C89" s="70" t="n"/>
+      <c r="D89" s="70" t="n"/>
+      <c r="E89" s="50" t="n"/>
+      <c r="F89" s="50" t="n"/>
+      <c r="G89" s="50" t="n"/>
+      <c r="H89" s="50" t="n"/>
+      <c r="I89" s="2" t="n"/>
+      <c r="J89" s="2" t="n"/>
+      <c r="K89" s="2" t="n"/>
+      <c r="L89" s="2" t="n"/>
+      <c r="M89" s="2" t="n"/>
+      <c r="N89" s="2" t="n"/>
+      <c r="O89" s="2" t="n"/>
+      <c r="P89" s="2" t="n"/>
+      <c r="Q89" s="2" t="n"/>
+      <c r="R89" s="2" t="n"/>
+      <c r="S89" s="2" t="n"/>
+      <c r="T89" s="2" t="n"/>
+    </row>
+    <row r="90" ht="27" customHeight="1">
+      <c r="A90" s="70" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="B90" s="70" t="n"/>
+      <c r="C90" s="70" t="n"/>
+      <c r="D90" s="70" t="n"/>
+      <c r="E90" s="50" t="n"/>
+      <c r="F90" s="50" t="n"/>
+      <c r="G90" s="50" t="n"/>
+      <c r="H90" s="50" t="n"/>
+      <c r="I90" s="2" t="n"/>
+      <c r="J90" s="2" t="n"/>
+      <c r="K90" s="2" t="n"/>
+      <c r="L90" s="2" t="n"/>
+      <c r="M90" s="2" t="n"/>
+      <c r="N90" s="2" t="n"/>
+      <c r="O90" s="2" t="n"/>
+      <c r="P90" s="2" t="n"/>
+      <c r="Q90" s="2" t="n"/>
+      <c r="R90" s="2" t="n"/>
+      <c r="S90" s="2" t="n"/>
+      <c r="T90" s="2" t="n"/>
+    </row>
+    <row r="91" ht="27" customHeight="1">
+      <c r="A91" s="2" t="n"/>
+      <c r="B91" s="109" t="n"/>
+      <c r="C91" s="2" t="n"/>
+      <c r="D91" s="2" t="n"/>
+      <c r="E91" s="52" t="n"/>
+      <c r="F91" s="2" t="n"/>
+      <c r="G91" s="26" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="H91" s="52" t="n"/>
+      <c r="I91" s="2" t="n"/>
+      <c r="J91" s="2" t="n"/>
+      <c r="K91" s="2" t="n"/>
+      <c r="L91" s="2" t="n"/>
+      <c r="M91" s="2" t="n"/>
+      <c r="N91" s="2" t="n"/>
+      <c r="O91" s="2" t="n"/>
+      <c r="P91" s="2" t="n"/>
+      <c r="Q91" s="2" t="n"/>
+      <c r="R91" s="2" t="n"/>
+      <c r="S91" s="2" t="n"/>
+      <c r="T91" s="2" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="80">
@@ -5044,75 +5246,75 @@
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A74:B74"/>
     <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C74"/>
-    <mergeCell ref="E58:E71"/>
+    <mergeCell ref="I58:I59"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="F56:G56"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C75"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A59:B59"/>
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="E23:E52"/>
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="C56:C57"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C73"/>
+    <mergeCell ref="A88:D88"/>
     <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A58:B59"/>
     <mergeCell ref="J21:J22"/>
+    <mergeCell ref="E60:E73"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="E58:E59"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A49:B49"/>
-    <mergeCell ref="H56:H57"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A3:I3"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="B87:D87"/>
     <mergeCell ref="A69:B69"/>
     <mergeCell ref="F21:G21"/>
+    <mergeCell ref="A78:B78"/>
     <mergeCell ref="A65:B65"/>
     <mergeCell ref="A5:I5"/>
+    <mergeCell ref="C78"/>
     <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A75:B75"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="C54"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="J58:J59"/>
     <mergeCell ref="A38:B38"/>
-    <mergeCell ref="E56:E57"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A56:B57"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="H21:H22"/>
+    <mergeCell ref="C74:D74"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D56:D57"/>
     <mergeCell ref="I21:I22"/>
     <mergeCell ref="A66:B66"/>
     <mergeCell ref="A50:B50"/>
-    <mergeCell ref="J56:J57"/>
-    <mergeCell ref="B79:D79"/>
     <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="F58:G58"/>
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C72:D72"/>
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A58:B58"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>